<commit_message>
Adding the code for create interaction
</commit_message>
<xml_diff>
--- a/src/main/resources/template-testing.xlsx
+++ b/src/main/resources/template-testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16236" windowHeight="7860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16116" windowHeight="7860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -114,13 +114,55 @@
   </si>
   <si>
     <t>iphone xs</t>
+  </si>
+  <si>
+    <t>newentityitem</t>
+  </si>
+  <si>
+    <t>Synonym</t>
+  </si>
+  <si>
+    <t>newEntityTitle</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>empnames</t>
+  </si>
+  <si>
+    <t>vidya</t>
+  </si>
+  <si>
+    <t>template title</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>Internet was slow in my mobile</t>
+  </si>
+  <si>
+    <t>text answer</t>
+  </si>
+  <si>
+    <t>Can you please provide me your mobile number</t>
+  </si>
+  <si>
+    <t>template Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet </t>
+  </si>
+  <si>
+    <t>Slow Internet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -145,6 +187,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -208,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -229,6 +277,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -589,9 +638,13 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -604,8 +657,29 @@
       <c r="D1" t="s">
         <v>29</v>
       </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -617,6 +691,27 @@
       </c>
       <c r="D2" t="s">
         <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -624,6 +719,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>